<commit_message>
Update Events page and test
</commit_message>
<xml_diff>
--- a/Test Data/PEMC Test Data.xlsx
+++ b/Test Data/PEMC Test Data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="149">
   <si>
     <t>Username</t>
   </si>
@@ -351,6 +351,21 @@
     <t xml:space="preserve">The quick, brown fox jumps over a lazy dog. DJs flock by when MTV ax quiz prog. </t>
   </si>
   <si>
+    <t>02/12/2020 07:00</t>
+  </si>
+  <si>
+    <t>02/13/2020 17:00</t>
+  </si>
+  <si>
+    <t>01/25/2020 07:00</t>
+  </si>
+  <si>
+    <t>01/30/2020 23:59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/14/2020 10:00 </t>
+  </si>
+  <si>
     <t>Please fill all required(*) fields.</t>
   </si>
   <si>
@@ -364,6 +379,93 @@
   </si>
   <si>
     <t>Lifetime</t>
+  </si>
+  <si>
+    <t>01/25/2020 07:01</t>
+  </si>
+  <si>
+    <t>01/25/2020 07:02</t>
+  </si>
+  <si>
+    <t>01/25/2020 07:03</t>
+  </si>
+  <si>
+    <t>01/25/2020 07:04</t>
+  </si>
+  <si>
+    <t>01/25/2020 07:05</t>
+  </si>
+  <si>
+    <t>01/25/2020 07:06</t>
+  </si>
+  <si>
+    <t>01/25/2020 07:07</t>
+  </si>
+  <si>
+    <t>01/25/2020 07:08</t>
+  </si>
+  <si>
+    <t>01/25/2020 07:09</t>
+  </si>
+  <si>
+    <t>01/25/2020 07:10</t>
+  </si>
+  <si>
+    <t>01/25/2020 07:11</t>
+  </si>
+  <si>
+    <t>01/25/2020 07:12</t>
+  </si>
+  <si>
+    <t>01/25/2020 07:13</t>
+  </si>
+  <si>
+    <t>01/25/2020 07:14</t>
+  </si>
+  <si>
+    <t>01/25/2020 07:15</t>
+  </si>
+  <si>
+    <t>01/25/2020 07:16</t>
+  </si>
+  <si>
+    <t>01/25/2020 07:17</t>
+  </si>
+  <si>
+    <t>01/25/2020 07:18</t>
+  </si>
+  <si>
+    <t>01/25/2020 07:19</t>
+  </si>
+  <si>
+    <t>01/25/2020 07:20</t>
+  </si>
+  <si>
+    <t>01/25/2020 07:21</t>
+  </si>
+  <si>
+    <t>01/25/2020 07:22</t>
+  </si>
+  <si>
+    <t>01/25/2020 07:23</t>
+  </si>
+  <si>
+    <t>01/25/2020 07:24</t>
+  </si>
+  <si>
+    <t>01/25/2020 07:25</t>
+  </si>
+  <si>
+    <t>01/25/2020 07:26</t>
+  </si>
+  <si>
+    <t>01/25/2020 07:27</t>
+  </si>
+  <si>
+    <t>01/25/2020 07:28</t>
+  </si>
+  <si>
+    <t>01/25/2020 07:29</t>
   </si>
 </sst>
 </file>
@@ -371,10 +473,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -394,29 +496,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -430,6 +510,43 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -439,14 +556,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -476,6 +594,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -483,24 +624,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -513,29 +638,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -546,7 +648,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -558,19 +744,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -582,151 +828,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -809,15 +911,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -844,6 +937,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -855,7 +957,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -873,130 +975,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1949,10 +2051,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:T32"/>
+  <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A33" sqref="$A33:$XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="31" customHeight="1"/>
@@ -2046,16 +2148,16 @@
         <v>63</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>102</v>
@@ -2065,7 +2167,7 @@
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>104</v>
@@ -2086,49 +2188,47 @@
         <v>87</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:20">
       <c r="A3" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="J3" s="2" t="s">
         <v>102</v>
       </c>
       <c r="K3" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>103</v>
-      </c>
+      <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2" t="s">
         <v>105</v>
@@ -2146,49 +2246,47 @@
         <v>87</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:20">
       <c r="A4" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="H4" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="J4" s="2" t="s">
         <v>102</v>
       </c>
       <c r="K4" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>103</v>
-      </c>
+      <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2" t="s">
         <v>105</v>
@@ -2206,49 +2304,47 @@
         <v>87</v>
       </c>
       <c r="T4" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:20">
       <c r="A5" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="H5" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="J5" s="2" t="s">
         <v>102</v>
       </c>
       <c r="K5" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>103</v>
-      </c>
+      <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2" t="s">
         <v>105</v>
@@ -2266,49 +2362,47 @@
         <v>87</v>
       </c>
       <c r="T5" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:20">
       <c r="A6" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="H6" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="J6" s="2" t="s">
         <v>102</v>
       </c>
       <c r="K6" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="L6" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>103</v>
-      </c>
+      <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2" t="s">
         <v>105</v>
@@ -2326,7 +2420,7 @@
         <v>87</v>
       </c>
       <c r="T6" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:20">
@@ -2340,22 +2434,22 @@
         <v>61</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>102</v>
@@ -2365,7 +2459,7 @@
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>104</v>
@@ -2386,49 +2480,47 @@
         <v>87</v>
       </c>
       <c r="T7" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:20">
       <c r="A8" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="H8" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="J8" s="2" t="s">
         <v>102</v>
       </c>
       <c r="K8" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="L8" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>103</v>
-      </c>
+      <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2" t="s">
         <v>105</v>
@@ -2446,49 +2538,47 @@
         <v>87</v>
       </c>
       <c r="T8" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:20">
       <c r="A9" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="H9" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="J9" s="2" t="s">
         <v>102</v>
       </c>
       <c r="K9" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="L9" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>103</v>
-      </c>
+      <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2" t="s">
         <v>105</v>
@@ -2506,7 +2596,7 @@
         <v>87</v>
       </c>
       <c r="T9" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="1:20">
@@ -2520,22 +2610,22 @@
         <v>61</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>102</v>
@@ -2545,7 +2635,7 @@
       </c>
       <c r="L10" s="2"/>
       <c r="M10" s="2" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>104</v>
@@ -2566,7 +2656,7 @@
         <v>87</v>
       </c>
       <c r="T10" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:20">
@@ -2580,22 +2670,22 @@
         <v>61</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>102</v>
@@ -2605,7 +2695,7 @@
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>104</v>
@@ -2626,49 +2716,47 @@
         <v>87</v>
       </c>
       <c r="T11" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" customHeight="1" spans="1:20">
       <c r="A12" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="H12" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="J12" s="2" t="s">
         <v>102</v>
       </c>
       <c r="K12" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="L12" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>103</v>
-      </c>
+      <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2" t="s">
         <v>105</v>
@@ -2686,49 +2774,47 @@
         <v>87</v>
       </c>
       <c r="T12" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:20">
       <c r="A13" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="3" t="s">
+      <c r="H13" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="J13" s="2" t="s">
         <v>102</v>
       </c>
       <c r="K13" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L13" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="L13" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>103</v>
-      </c>
+      <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2" t="s">
         <v>105</v>
@@ -2746,49 +2832,47 @@
         <v>87</v>
       </c>
       <c r="T13" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" customHeight="1" spans="1:20">
       <c r="A14" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14" s="3" t="s">
+      <c r="H14" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="J14" s="2" t="s">
         <v>102</v>
       </c>
       <c r="K14" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L14" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="L14" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>103</v>
-      </c>
+      <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2" t="s">
         <v>105</v>
@@ -2806,49 +2890,47 @@
         <v>87</v>
       </c>
       <c r="T14" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" customHeight="1" spans="1:20">
       <c r="A15" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" s="3" t="s">
+      <c r="H15" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="J15" s="2" t="s">
         <v>102</v>
       </c>
       <c r="K15" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L15" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="L15" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>103</v>
-      </c>
+      <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2" t="s">
         <v>105</v>
@@ -2866,7 +2948,7 @@
         <v>87</v>
       </c>
       <c r="T15" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" customHeight="1" spans="1:20">
@@ -2880,22 +2962,22 @@
         <v>61</v>
       </c>
       <c r="D16" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>102</v>
@@ -2905,7 +2987,7 @@
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>104</v>
@@ -2926,49 +3008,47 @@
         <v>87</v>
       </c>
       <c r="T16" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" customHeight="1" spans="1:20">
       <c r="A17" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="3" t="s">
+      <c r="H17" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="I17" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="J17" s="2" t="s">
         <v>102</v>
       </c>
       <c r="K17" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="L17" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>103</v>
-      </c>
+      <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2" t="s">
         <v>105</v>
@@ -2986,49 +3066,47 @@
         <v>87</v>
       </c>
       <c r="T17" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" customHeight="1" spans="1:20">
       <c r="A18" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="3" t="s">
+      <c r="H18" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="I18" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="J18" s="2" t="s">
         <v>102</v>
       </c>
       <c r="K18" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L18" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="L18" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>103</v>
-      </c>
+      <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2" t="s">
         <v>105</v>
@@ -3046,7 +3124,7 @@
         <v>87</v>
       </c>
       <c r="T18" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" customHeight="1" spans="1:20">
@@ -3060,22 +3138,22 @@
         <v>61</v>
       </c>
       <c r="D19" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="I19" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>102</v>
@@ -3085,7 +3163,7 @@
       </c>
       <c r="L19" s="2"/>
       <c r="M19" s="2" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>104</v>
@@ -3106,49 +3184,47 @@
         <v>87</v>
       </c>
       <c r="T19" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" customHeight="1" spans="1:20">
       <c r="A20" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" s="3" t="s">
+      <c r="H20" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="I20" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="J20" s="2" t="s">
         <v>102</v>
       </c>
       <c r="K20" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L20" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="L20" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="M20" s="2" t="s">
-        <v>103</v>
-      </c>
+      <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2" t="s">
         <v>105</v>
@@ -3166,49 +3242,47 @@
         <v>87</v>
       </c>
       <c r="T20" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" customHeight="1" spans="1:20">
       <c r="A21" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" s="3" t="s">
+      <c r="H21" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="I21" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="J21" s="2" t="s">
         <v>102</v>
       </c>
       <c r="K21" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L21" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="L21" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>103</v>
-      </c>
+      <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2" t="s">
         <v>105</v>
@@ -3226,7 +3300,7 @@
         <v>87</v>
       </c>
       <c r="T21" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" customHeight="1" spans="1:20">
@@ -3240,22 +3314,22 @@
         <v>61</v>
       </c>
       <c r="D22" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>102</v>
@@ -3265,7 +3339,7 @@
       </c>
       <c r="L22" s="2"/>
       <c r="M22" s="2" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="N22" s="2" t="s">
         <v>104</v>
@@ -3286,7 +3360,7 @@
         <v>87</v>
       </c>
       <c r="T22" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" customHeight="1" spans="1:20">
@@ -3300,22 +3374,22 @@
         <v>61</v>
       </c>
       <c r="D23" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="I23" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>102</v>
@@ -3325,7 +3399,7 @@
       </c>
       <c r="L23" s="2"/>
       <c r="M23" s="2" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="N23" s="2" t="s">
         <v>104</v>
@@ -3346,7 +3420,7 @@
         <v>87</v>
       </c>
       <c r="T23" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" customHeight="1" spans="1:20">
@@ -3360,22 +3434,22 @@
         <v>61</v>
       </c>
       <c r="D24" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="I24" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>102</v>
@@ -3385,7 +3459,7 @@
       </c>
       <c r="L24" s="2"/>
       <c r="M24" s="2" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="N24" s="2" t="s">
         <v>104</v>
@@ -3406,48 +3480,48 @@
         <v>87</v>
       </c>
       <c r="T24" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" customHeight="1" spans="1:20">
       <c r="A25" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D25" s="3" t="s">
+      <c r="H25" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="I25" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="J25" s="2" t="s">
         <v>102</v>
       </c>
       <c r="K25" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L25" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="L25" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="M25" s="2" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" s="2" t="s">
@@ -3466,49 +3540,47 @@
         <v>87</v>
       </c>
       <c r="T25" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" customHeight="1" spans="1:20">
       <c r="A26" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D26" s="3" t="s">
+      <c r="H26" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I26" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="J26" s="2" t="s">
         <v>102</v>
       </c>
       <c r="K26" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L26" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="L26" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>103</v>
-      </c>
+      <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2" t="s">
         <v>105</v>
@@ -3526,49 +3598,47 @@
         <v>87</v>
       </c>
       <c r="T26" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" customHeight="1" spans="1:20">
       <c r="A27" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" s="3" t="s">
+      <c r="H27" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I27" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="J27" s="2" t="s">
         <v>102</v>
       </c>
       <c r="K27" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L27" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="L27" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="M27" s="2" t="s">
-        <v>103</v>
-      </c>
+      <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2" t="s">
         <v>105</v>
@@ -3586,7 +3656,7 @@
         <v>87</v>
       </c>
       <c r="T27" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" customHeight="1" spans="1:20">
@@ -3600,22 +3670,22 @@
         <v>61</v>
       </c>
       <c r="D28" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I28" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>102</v>
@@ -3625,7 +3695,7 @@
       </c>
       <c r="L28" s="2"/>
       <c r="M28" s="2" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="N28" s="2" t="s">
         <v>104</v>
@@ -3646,7 +3716,7 @@
         <v>87</v>
       </c>
       <c r="T28" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" customHeight="1" spans="1:20">
@@ -3660,22 +3730,22 @@
         <v>61</v>
       </c>
       <c r="D29" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="I29" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>102</v>
@@ -3685,7 +3755,7 @@
       </c>
       <c r="L29" s="2"/>
       <c r="M29" s="2" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="N29" s="2" t="s">
         <v>104</v>
@@ -3706,7 +3776,7 @@
         <v>87</v>
       </c>
       <c r="T29" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" customHeight="1" spans="1:20">
@@ -3720,22 +3790,22 @@
         <v>61</v>
       </c>
       <c r="D30" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I30" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>102</v>
@@ -3745,7 +3815,7 @@
       </c>
       <c r="L30" s="2"/>
       <c r="M30" s="2" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="N30" s="2" t="s">
         <v>104</v>
@@ -3766,49 +3836,47 @@
         <v>87</v>
       </c>
       <c r="T30" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" customHeight="1" spans="1:20">
       <c r="A31" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G31" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D31" s="3" t="s">
+      <c r="H31" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="I31" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="J31" s="2" t="s">
         <v>102</v>
       </c>
       <c r="K31" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L31" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="L31" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="M31" s="2" t="s">
-        <v>103</v>
-      </c>
+      <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2" t="s">
         <v>105</v>
@@ -3826,49 +3894,47 @@
         <v>87</v>
       </c>
       <c r="T31" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" customHeight="1" spans="1:20">
       <c r="A32" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G32" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D32" s="3" t="s">
+      <c r="H32" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="I32" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="J32" s="2" t="s">
         <v>102</v>
       </c>
       <c r="K32" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L32" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="L32" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="M32" s="2" t="s">
-        <v>103</v>
-      </c>
+      <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" s="2" t="s">
         <v>105</v>
@@ -3886,7 +3952,67 @@
         <v>87</v>
       </c>
       <c r="T32" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" customHeight="1" spans="1:20">
+      <c r="A33" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>110</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="O33" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P33" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q33" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="R33" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="S33" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="T33" s="6" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -4029,21 +4155,21 @@
         <v>87</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" ht="285" spans="1:20">
       <c r="A3" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>63</v>
@@ -4064,7 +4190,7 @@
         <v>102</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>103</v>
@@ -4089,21 +4215,21 @@
         <v>87</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" ht="285" spans="1:20">
       <c r="A4" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>63</v>
@@ -4124,7 +4250,7 @@
         <v>102</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>103</v>
@@ -4149,21 +4275,21 @@
         <v>87</v>
       </c>
       <c r="T4" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" ht="285" spans="1:20">
       <c r="A5" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>63</v>
@@ -4184,7 +4310,7 @@
         <v>102</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>103</v>
@@ -4209,21 +4335,21 @@
         <v>87</v>
       </c>
       <c r="T5" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" ht="285" spans="1:20">
       <c r="A6" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>63</v>
@@ -4244,7 +4370,7 @@
         <v>102</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>103</v>
@@ -4269,7 +4395,7 @@
         <v>87</v>
       </c>
       <c r="T6" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" ht="285" spans="1:20">
@@ -4283,7 +4409,7 @@
         <v>61</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>63</v>
@@ -4329,21 +4455,21 @@
         <v>87</v>
       </c>
       <c r="T7" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" ht="285" spans="1:20">
       <c r="A8" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>63</v>
@@ -4364,7 +4490,7 @@
         <v>102</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>103</v>
@@ -4389,21 +4515,21 @@
         <v>87</v>
       </c>
       <c r="T8" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" ht="285" spans="1:20">
       <c r="A9" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>63</v>
@@ -4424,7 +4550,7 @@
         <v>102</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>103</v>
@@ -4449,7 +4575,7 @@
         <v>87</v>
       </c>
       <c r="T9" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" ht="285" spans="1:20">
@@ -4463,7 +4589,7 @@
         <v>61</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>63</v>
@@ -4509,7 +4635,7 @@
         <v>87</v>
       </c>
       <c r="T10" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" ht="285" spans="1:20">
@@ -4523,7 +4649,7 @@
         <v>61</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>63</v>
@@ -4569,21 +4695,21 @@
         <v>87</v>
       </c>
       <c r="T11" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" ht="285" spans="1:20">
       <c r="A12" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>63</v>
@@ -4604,7 +4730,7 @@
         <v>102</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>103</v>
@@ -4629,21 +4755,21 @@
         <v>87</v>
       </c>
       <c r="T12" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" ht="69" customHeight="1" spans="1:20">
       <c r="A13" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>63</v>
@@ -4664,7 +4790,7 @@
         <v>102</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>103</v>
@@ -4689,21 +4815,21 @@
         <v>87</v>
       </c>
       <c r="T13" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" ht="285" spans="1:20">
       <c r="A14" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>63</v>
@@ -4724,7 +4850,7 @@
         <v>102</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>103</v>
@@ -4749,21 +4875,21 @@
         <v>87</v>
       </c>
       <c r="T14" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" ht="285" spans="1:20">
       <c r="A15" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>63</v>
@@ -4784,7 +4910,7 @@
         <v>102</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>103</v>
@@ -4809,7 +4935,7 @@
         <v>87</v>
       </c>
       <c r="T15" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" ht="285" spans="1:20">
@@ -4823,7 +4949,7 @@
         <v>61</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>63</v>
@@ -4869,21 +4995,21 @@
         <v>87</v>
       </c>
       <c r="T16" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" ht="285" spans="1:20">
       <c r="A17" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>63</v>
@@ -4904,7 +5030,7 @@
         <v>102</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>103</v>
@@ -4929,21 +5055,21 @@
         <v>87</v>
       </c>
       <c r="T17" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" ht="285" spans="1:20">
       <c r="A18" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>63</v>
@@ -4964,7 +5090,7 @@
         <v>102</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>103</v>
@@ -4989,7 +5115,7 @@
         <v>87</v>
       </c>
       <c r="T18" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" ht="285" spans="1:20">
@@ -5003,7 +5129,7 @@
         <v>61</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>63</v>
@@ -5049,21 +5175,21 @@
         <v>87</v>
       </c>
       <c r="T19" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" ht="285" spans="1:20">
       <c r="A20" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>63</v>
@@ -5084,7 +5210,7 @@
         <v>102</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>103</v>
@@ -5109,21 +5235,21 @@
         <v>87</v>
       </c>
       <c r="T20" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" ht="285" spans="1:20">
       <c r="A21" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>63</v>
@@ -5144,7 +5270,7 @@
         <v>102</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>103</v>
@@ -5169,7 +5295,7 @@
         <v>87</v>
       </c>
       <c r="T21" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" ht="285" spans="1:20">
@@ -5183,7 +5309,7 @@
         <v>61</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>63</v>
@@ -5229,7 +5355,7 @@
         <v>87</v>
       </c>
       <c r="T22" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" ht="285" spans="1:20">
@@ -5243,7 +5369,7 @@
         <v>61</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>63</v>
@@ -5289,7 +5415,7 @@
         <v>87</v>
       </c>
       <c r="T23" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" ht="285" spans="1:20">
@@ -5303,7 +5429,7 @@
         <v>61</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>63</v>
@@ -5349,21 +5475,21 @@
         <v>87</v>
       </c>
       <c r="T24" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" ht="285" spans="1:20">
       <c r="A25" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>63</v>
@@ -5384,7 +5510,7 @@
         <v>102</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>103</v>
@@ -5409,21 +5535,21 @@
         <v>87</v>
       </c>
       <c r="T25" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" ht="285" spans="1:20">
       <c r="A26" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>63</v>
@@ -5444,7 +5570,7 @@
         <v>102</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>103</v>
@@ -5469,21 +5595,21 @@
         <v>87</v>
       </c>
       <c r="T26" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" ht="285" spans="1:20">
       <c r="A27" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>63</v>
@@ -5504,7 +5630,7 @@
         <v>102</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>103</v>
@@ -5529,7 +5655,7 @@
         <v>87</v>
       </c>
       <c r="T27" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" ht="285" spans="1:20">
@@ -5543,7 +5669,7 @@
         <v>61</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>63</v>
@@ -5589,7 +5715,7 @@
         <v>87</v>
       </c>
       <c r="T28" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" ht="285" spans="1:20">
@@ -5603,7 +5729,7 @@
         <v>61</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>63</v>
@@ -5649,7 +5775,7 @@
         <v>87</v>
       </c>
       <c r="T29" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" ht="285" spans="1:20">
@@ -5663,7 +5789,7 @@
         <v>61</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>63</v>
@@ -5709,21 +5835,21 @@
         <v>87</v>
       </c>
       <c r="T30" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" ht="285" spans="1:20">
       <c r="A31" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>63</v>
@@ -5744,7 +5870,7 @@
         <v>102</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="L31" s="2" t="s">
         <v>103</v>
@@ -5769,21 +5895,21 @@
         <v>87</v>
       </c>
       <c r="T31" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" ht="285" spans="1:20">
       <c r="A32" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>63</v>
@@ -5804,7 +5930,7 @@
         <v>102</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="L32" s="2" t="s">
         <v>103</v>
@@ -5829,7 +5955,7 @@
         <v>87</v>
       </c>
       <c r="T32" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>